<commit_message>
PC & D sheet Done
</commit_message>
<xml_diff>
--- a/backend/server/final_report.xlsx
+++ b/backend/server/final_report.xlsx
@@ -14,6 +14,7 @@
     <sheet name="SS-C1" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="SS-C2" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="SS-D" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="SS-D1" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -82,27 +83,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -470,7 +486,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:J11"/>
+  <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +503,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Statement</t>
+          <t>Statement-1</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -497,34 +513,38 @@
       </c>
       <c r="C2" s="2" t="n"/>
       <c r="D2" s="2" t="n"/>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>Term Loan Computation</t>
         </is>
       </c>
+      <c r="G2" s="2" t="n"/>
+      <c r="H2" s="2" t="n"/>
+      <c r="I2" s="2" t="n"/>
+      <c r="J2" s="2" t="n"/>
     </row>
     <row r="3" ht="32" customHeight="1">
       <c r="A3" s="2" t="inlineStr"/>
       <c r="B3" s="2" t="inlineStr"/>
       <c r="C3" s="2" t="inlineStr"/>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs</t>
         </is>
       </c>
-      <c r="F3" s="5" t="inlineStr"/>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="F3" s="4" t="inlineStr"/>
+      <c r="G3" s="4" t="inlineStr">
         <is>
           <t>Rs Lakhs</t>
         </is>
       </c>
-      <c r="H3" s="6" t="inlineStr">
+      <c r="H3" s="5" t="inlineStr">
         <is>
           <t>% of Contribution to Margin Money</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr"/>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="I3" s="4" t="inlineStr"/>
+      <c r="J3" s="4" t="inlineStr">
         <is>
           <t>Term Loan</t>
         </is>
@@ -535,6 +555,11 @@
       <c r="B4" s="2" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="2" t="n"/>
+      <c r="F4" s="2" t="n"/>
+      <c r="G4" s="2" t="n"/>
+      <c r="H4" s="2" t="n"/>
+      <c r="I4" s="2" t="n"/>
+      <c r="J4" s="2" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -542,14 +567,29 @@
           <t>Land</t>
         </is>
       </c>
-      <c r="B5" s="4" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>SS-A</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr"/>
       <c r="D5" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>Land</t>
+        </is>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="H5" s="7" t="n">
         <v>1</v>
+      </c>
+      <c r="I5" s="2" t="n"/>
+      <c r="J5" s="8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -558,14 +598,29 @@
           <t>Building</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>SS-B</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr"/>
       <c r="D6" s="2" t="n">
-        <v>1</v>
+        <v>2.2</v>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>Building</t>
+        </is>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I6" s="2" t="n"/>
+      <c r="J6" s="8" t="n">
+        <v>1.65</v>
       </c>
     </row>
     <row r="7">
@@ -574,14 +629,29 @@
           <t>Plant &amp; Equipment</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>SS-C</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr"/>
       <c r="D7" s="2" t="n">
-        <v>1</v>
+        <v>2.4</v>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>Plant &amp; Equipments</t>
+        </is>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I7" s="2" t="n"/>
+      <c r="J7" s="8" t="n">
+        <v>1.8</v>
       </c>
     </row>
     <row r="8">
@@ -590,7 +660,7 @@
           <t>Furniture &amp; Fittings</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>SS-C1</t>
         </is>
@@ -599,6 +669,21 @@
       <c r="D8" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>Furniture &amp; Fittings</t>
+        </is>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I8" s="2" t="n"/>
+      <c r="J8" s="8" t="n">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
@@ -606,14 +691,29 @@
           <t>Electrical Fittings</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>SS-C2</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr"/>
       <c r="D9" s="2" t="n">
-        <v>1</v>
+        <v>3.2</v>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>Electrical Fittings</t>
+        </is>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I9" s="2" t="n"/>
+      <c r="J9" s="8" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="10">
@@ -622,14 +722,29 @@
           <t>Other Fixed Assets</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>SS-C3</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr"/>
       <c r="D10" s="2" t="n">
-        <v>1</v>
+        <v>2.2</v>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>Other Fixed Assets</t>
+        </is>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I10" s="2" t="n"/>
+      <c r="J10" s="8" t="n">
+        <v>1.65</v>
       </c>
     </row>
     <row r="11">
@@ -638,18 +753,143 @@
           <t>Preoperative expenses</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>SS-D</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr"/>
       <c r="D11" s="2" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>Preoperative Expenses</t>
+        </is>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="H11" s="7" t="n">
         <v>1</v>
       </c>
+      <c r="I11" s="2" t="n"/>
+      <c r="J11" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n"/>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
+      <c r="D12" s="2" t="n"/>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>23.74</v>
+      </c>
+      <c r="H12" s="1" t="inlineStr"/>
+      <c r="I12" s="1" t="inlineStr"/>
+      <c r="J12" s="1" t="n">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B13" s="9" t="inlineStr"/>
+      <c r="C13" s="9" t="inlineStr"/>
+      <c r="D13" s="9" t="n">
+        <v>23.74</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n"/>
+      <c r="B14" s="2" t="n"/>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>Statement-2</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>Means of Finance</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr"/>
+      <c r="B16" s="2" t="inlineStr"/>
+      <c r="C16" s="2" t="inlineStr"/>
+      <c r="D16" s="10" t="inlineStr">
+        <is>
+          <t>Rs Lakhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n"/>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Equity</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr"/>
+      <c r="C18" s="2" t="inlineStr"/>
+      <c r="D18" s="8" t="n">
+        <v>15.49</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>Debt</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr"/>
+      <c r="C19" s="2" t="inlineStr"/>
+      <c r="D19" s="8" t="n">
+        <v>8.25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n"/>
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B21" s="9" t="inlineStr"/>
+      <c r="C21" s="9" t="inlineStr"/>
+      <c r="D21" s="11" t="n">
+        <v>23.74</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:J2"/>
   </mergeCells>
@@ -663,7 +903,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:E6"/>
+  <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -681,7 +921,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement A</t>
         </is>
@@ -696,27 +936,27 @@
       <c r="E2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Sq-Ft</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/ Sq-Ft</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs</t>
         </is>
@@ -730,35 +970,54 @@
       <c r="E4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n">
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9" t="n">
-        <v>1</v>
+      <c r="D5" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr"/>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="A6" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr"/>
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C6" s="1" t="inlineStr"/>
-      <c r="D6" s="1" t="inlineStr"/>
-      <c r="E6" s="1" t="n">
-        <v>1</v>
+      <c r="C7" s="1" t="inlineStr"/>
+      <c r="D7" s="1" t="inlineStr"/>
+      <c r="E7" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -793,7 +1052,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement B</t>
         </is>
@@ -808,27 +1067,27 @@
       <c r="E2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Sq-Ft</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/ Sq-Ft</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs</t>
         </is>
@@ -842,22 +1101,22 @@
       <c r="E4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" s="9" t="n">
-        <v>1</v>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="13" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E5" s="13" t="n">
+        <v>2.2</v>
       </c>
     </row>
     <row r="6">
@@ -870,7 +1129,7 @@
       <c r="C6" s="1" t="inlineStr"/>
       <c r="D6" s="1" t="inlineStr"/>
       <c r="E6" s="1" t="n">
-        <v>1</v>
+        <v>2.2</v>
       </c>
     </row>
   </sheetData>
@@ -901,7 +1160,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement C</t>
         </is>
@@ -914,17 +1173,17 @@
       <c r="C2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/Nos</t>
         </is>
@@ -936,16 +1195,16 @@
       <c r="C4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n">
-        <v>1</v>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>2.4</v>
       </c>
     </row>
     <row r="6">
@@ -956,7 +1215,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1</v>
+        <v>2.4</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +1246,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement C1</t>
         </is>
@@ -1000,17 +1259,17 @@
       <c r="C2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/Nos</t>
         </is>
@@ -1022,15 +1281,15 @@
       <c r="C4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n">
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1073,7 +1332,7 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement C2</t>
         </is>
@@ -1086,17 +1345,17 @@
       <c r="C2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/Nos</t>
         </is>
@@ -1108,16 +1367,16 @@
       <c r="C4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n">
-        <v>1</v>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>3.2</v>
       </c>
     </row>
     <row r="6">
@@ -1128,7 +1387,7 @@
         </is>
       </c>
       <c r="C6" s="1" t="n">
-        <v>1</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="7">
@@ -1137,7 +1396,7 @@
       <c r="C7" s="2" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="inlineStr">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement C3</t>
         </is>
@@ -1150,17 +1409,17 @@
       <c r="C8" s="2" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="inlineStr">
+      <c r="A9" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/Nos</t>
         </is>
@@ -1172,16 +1431,16 @@
       <c r="C10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C11" s="9" t="n">
-        <v>1</v>
+      <c r="B11" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C11" s="13" t="n">
+        <v>2.2</v>
       </c>
     </row>
     <row r="12">
@@ -1192,7 +1451,7 @@
         </is>
       </c>
       <c r="C12" s="1" t="n">
-        <v>1</v>
+        <v>2.2</v>
       </c>
     </row>
   </sheetData>
@@ -1210,7 +1469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1219,12 +1478,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="47" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>Sub-Statement D</t>
         </is>
@@ -1237,17 +1496,17 @@
       <c r="C2" s="2" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="inlineStr">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>SI.No</t>
         </is>
       </c>
-      <c r="B3" s="4" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Particulars</t>
         </is>
       </c>
-      <c r="C3" s="4" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Rs Lakhs/Nos</t>
         </is>
@@ -1259,27 +1518,53 @@
       <c r="C4" s="2" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>inp1</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="n">
-        <v>1</v>
+      <c r="B5" s="12" t="inlineStr">
+        <is>
+          <t>input</t>
+        </is>
+      </c>
+      <c r="C5" s="13" t="n">
+        <v>3.1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr"/>
-      <c r="B6" s="1" t="inlineStr">
+      <c r="A6" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="inlineStr">
+        <is>
+          <t>input2</t>
+        </is>
+      </c>
+      <c r="C6" s="13" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="inlineStr">
+        <is>
+          <t>Interest during construction period (SS-D1)</t>
+        </is>
+      </c>
+      <c r="C7" s="13" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr"/>
+      <c r="B8" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="C6" s="1" t="n">
-        <v>1</v>
+      <c r="C8" s="1" t="n">
+        <v>4.74</v>
       </c>
     </row>
   </sheetData>
@@ -1288,4 +1573,384 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A2:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>Sub-Statement D1</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>Interest During Construction Period</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" s="2" t="n"/>
+    </row>
+    <row r="3" ht="32" customHeight="1">
+      <c r="A3" s="5" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>% of Loan withdrawn during construction period</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>Loan amount withdrawn</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>Cumulative Amount Outstanding</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Interest</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n"/>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Rs Lakhs</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="E4" s="2" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr"/>
+      <c r="B5" s="2" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="C5" s="2" t="inlineStr"/>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="14" t="n">
+        <v>0.1375</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>2025-2026</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="n"/>
+      <c r="E6" s="2" t="n"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>JUNE</t>
+        </is>
+      </c>
+      <c r="B7" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>JULY</t>
+        </is>
+      </c>
+      <c r="B8" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>AUGUST</t>
+        </is>
+      </c>
+      <c r="B9" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>SEPTEMBER</t>
+        </is>
+      </c>
+      <c r="B10" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>OCTOBER</t>
+        </is>
+      </c>
+      <c r="B11" s="15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>NOVEMBER</t>
+        </is>
+      </c>
+      <c r="B12" s="15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>DECEMBER</t>
+        </is>
+      </c>
+      <c r="B13" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>JANUARY</t>
+        </is>
+      </c>
+      <c r="B14" s="15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>FEBRUARY</t>
+        </is>
+      </c>
+      <c r="B15" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>MARCH</t>
+        </is>
+      </c>
+      <c r="B16" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="inlineStr">
+        <is>
+          <t>2026-2027</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n"/>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n"/>
+      <c r="E17" s="2" t="n"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>APRIL</t>
+        </is>
+      </c>
+      <c r="B18" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>MAY</t>
+        </is>
+      </c>
+      <c r="B19" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>JUNE</t>
+        </is>
+      </c>
+      <c r="B20" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B21" s="16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="D21" s="1" t="n"/>
+      <c r="E21" s="1" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>